<commit_message>
Final commit before merge
</commit_message>
<xml_diff>
--- a/assets/sample_excel.xlsx
+++ b/assets/sample_excel.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Ranjeet Katiyal</t>
   </si>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t>should be only M or F</t>
-  </si>
-  <si>
-    <t>only 10 digits will be accepted. No +91 or 0 infront</t>
   </si>
 </sst>
 </file>
@@ -81,7 +78,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -97,12 +94,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCA4966"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -127,7 +118,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -192,53 +183,6 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>355600</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>368300</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="7" name="Straight Arrow Connector 6"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3594100" y="749300"/>
-          <a:ext cx="12700" cy="1181100"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
@@ -617,7 +561,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:C9"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -701,9 +645,7 @@
       <c r="C9" s="3"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="D11" s="4" t="s">
-        <v>12</v>
-      </c>
+      <c r="D11" s="4"/>
       <c r="E11" s="4"/>
     </row>
   </sheetData>
@@ -717,7 +659,6 @@
     <hyperlink ref="E3" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId4"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>